<commit_message>
Fix not selecting director button
</commit_message>
<xml_diff>
--- a/MovieDatabaseProcess/output-spreadsheets/director-gross-information.xlsx
+++ b/MovieDatabaseProcess/output-spreadsheets/director-gross-information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maggi\Documents\GitHub\rpa-solution\MovieDatabaseProcess\output-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFF07E1-25C1-437A-A589-3E0D87B31C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF0F881-D6B8-4627-A0B7-76810F6C5BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13260" yWindow="2895" windowWidth="11400" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,14 +25,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Director</t>
+  </si>
   <si>
     <t>Movie</t>
   </si>
   <si>
-    <t>Director</t>
-  </si>
-  <si>
     <t>Worldwide Gross</t>
   </si>
   <si>
@@ -40,6 +40,24 @@
   </si>
   <si>
     <t>Thor: Love and Thunder</t>
+  </si>
+  <si>
+    <t>steven speilberg</t>
+  </si>
+  <si>
+    <t>West Side Story</t>
+  </si>
+  <si>
+    <t>james cameron</t>
+  </si>
+  <si>
+    <t>Duets</t>
+  </si>
+  <si>
+    <t>christopher nolan</t>
+  </si>
+  <si>
+    <t>Quay</t>
   </si>
 </sst>
 </file>
@@ -357,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
@@ -371,10 +389,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -389,6 +407,39 @@
       </c>
       <c r="C2">
         <v>759828739</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>76016171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>6620242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>51858</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use find children to solve issue
</commit_message>
<xml_diff>
--- a/MovieDatabaseProcess/output-spreadsheets/director-gross-information.xlsx
+++ b/MovieDatabaseProcess/output-spreadsheets/director-gross-information.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maggi\Documents\GitHub\rpa-solution\MovieDatabaseProcess\output-spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF0F881-D6B8-4627-A0B7-76810F6C5BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74406FDE-F75D-4271-B2C7-DB394BF6772A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13260" yWindow="2895" windowWidth="11400" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16440" yWindow="2085" windowWidth="11400" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>Director</t>
   </si>
@@ -45,19 +45,67 @@
     <t>steven speilberg</t>
   </si>
   <si>
-    <t>West Side Story</t>
-  </si>
-  <si>
     <t>james cameron</t>
   </si>
   <si>
-    <t>Duets</t>
-  </si>
-  <si>
     <t>christopher nolan</t>
   </si>
   <si>
-    <t>Quay</t>
+    <t>Avatar</t>
+  </si>
+  <si>
+    <t>Titanic</t>
+  </si>
+  <si>
+    <t>Jurassic Park</t>
+  </si>
+  <si>
+    <t>The Dark Knight Rises</t>
+  </si>
+  <si>
+    <t>The Dark Knight</t>
+  </si>
+  <si>
+    <t>Thor: Ragnarok</t>
+  </si>
+  <si>
+    <t>Inception</t>
+  </si>
+  <si>
+    <t>E.T. the Extra-Terrestrial</t>
+  </si>
+  <si>
+    <t>Indiana Jones and the Kingdom of the Crystal Skull</t>
+  </si>
+  <si>
+    <t>Interstellar</t>
+  </si>
+  <si>
+    <t>The Lost World: Jurassic Park</t>
+  </si>
+  <si>
+    <t>War of the Worlds</t>
+  </si>
+  <si>
+    <t>Dunkirk</t>
+  </si>
+  <si>
+    <t>Terminator 2: Judgment Day</t>
+  </si>
+  <si>
+    <t>True Lies</t>
+  </si>
+  <si>
+    <t>Aliens</t>
+  </si>
+  <si>
+    <t>Jojo Rabbit</t>
+  </si>
+  <si>
+    <t>Boy</t>
+  </si>
+  <si>
+    <t>Hunt for the Wilderpeople</t>
   </si>
 </sst>
 </file>
@@ -375,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
@@ -400,46 +448,222 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>759828739</v>
+        <v>2920357254</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3">
-        <v>76016171</v>
+        <v>2201647264</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>6620242</v>
+        <v>1109802321</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>51858</v>
+        <v>1081153097</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>1006234167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>853983879</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>836848102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>792910554</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>790653942</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>760677374</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12">
+        <v>716218351</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13">
+        <v>618638999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>603873119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>527016307</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>520881154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <v>378882411</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18">
+        <v>131060248</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19">
+        <v>90335025</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20">
+        <v>43551154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21">
+        <v>23915910</v>
       </c>
     </row>
   </sheetData>

</xml_diff>